<commit_message>
updated calculations for 57MHz pixel clock
</commit_message>
<xml_diff>
--- a/calculations/period_calculation.xlsx
+++ b/calculations/period_calculation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Galen\Documents\Code\miniscope_cypress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Documents\FEE\code\cyfxuvc_an75779\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -423,40 +423,39 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.53515625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="3" max="5" width="8.69140625" customWidth="1"/>
+    <col min="6" max="6" width="14.3046875" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" customWidth="1"/>
+    <col min="8" max="8" width="27.69140625" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="10" max="1025" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <f>113.75/2</f>
-        <v>56.875</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <f>10^9/(B1*10^6)</f>
-        <v>17.582417582417584</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17.543859649122808</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -468,25 +467,25 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6">
         <f>B2*C3*8/1000</f>
-        <v>15.472527472527474</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15.43859649122807</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
         <f>B6*(57/12)</f>
-        <v>73.494505494505503</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73.333333333333329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -496,32 +495,32 @@
       </c>
       <c r="C8">
         <f>C9/(B6*10^-6)</f>
-        <v>2154.3560606060605</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2159.090909090909</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
         <f>B8*B7/10^6</f>
-        <v>5.0123252747252753E-2</v>
+        <v>5.0013333333333326E-2</v>
       </c>
       <c r="C9">
         <f>1/C10</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B10">
         <f>1/B9</f>
-        <v>19.950820132175277</v>
+        <v>19.994668088509734</v>
       </c>
       <c r="C10">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -529,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -537,7 +536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -545,7 +544,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -553,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -563,14 +562,14 @@
       </c>
       <c r="C17">
         <f>B17*B6*10^-6</f>
-        <v>7.6589010989010992E-3</v>
+        <v>7.6421052631578945E-3</v>
       </c>
       <c r="D17">
         <f>1/C17</f>
-        <v>130.56703397612489</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>130.85399449035813</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -578,7 +577,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -586,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -594,7 +593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -602,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -611,7 +610,7 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -620,7 +619,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -630,28 +629,28 @@
       </c>
       <c r="C26">
         <f>B26*B6*10^-6</f>
-        <v>3.3405186813186813E-2</v>
+        <v>3.3331929824561402E-2</v>
       </c>
       <c r="D26">
         <f>1/C26</f>
-        <v>29.935470967198619</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30.001263211082573</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C27">
         <f>C26*10^9/100</f>
-        <v>334051.86813186813</v>
+        <v>333319.29824561405</v>
       </c>
       <c r="D27">
         <f>ROUND(C27,0)</f>
-        <v>334052</v>
+        <v>333319</v>
       </c>
       <c r="E27" t="str">
         <f>DEC2HEX(D27)</f>
-        <v>518E4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51607</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C28" t="s">
         <v>18</v>
       </c>
@@ -671,7 +670,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C29">
         <v>30</v>
       </c>
@@ -681,41 +680,41 @@
       </c>
       <c r="E29">
         <f>D29/(B6*10^-6)</f>
-        <v>2154.3560606060605</v>
+        <v>2159.090909090909</v>
       </c>
       <c r="F29">
         <f>ROUNDDOWN(E29,0)</f>
-        <v>2154</v>
+        <v>2159</v>
       </c>
       <c r="G29">
         <f>F29-1</f>
-        <v>2153</v>
+        <v>2158</v>
       </c>
       <c r="H29">
         <f>F29*B6*10^-6</f>
-        <v>3.3327824175824174E-2</v>
+        <v>3.3331929824561402E-2</v>
       </c>
       <c r="I29">
         <f>H29/10^-7</f>
-        <v>333278.24175824173</v>
+        <v>333319.29824561405</v>
       </c>
       <c r="J29">
         <f>ROUND(I29,0)</f>
-        <v>333278</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>333319</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="F30" t="str">
         <f>DEC2HEX(F29)</f>
-        <v>86A</v>
+        <v>86F</v>
       </c>
       <c r="G30" t="str">
         <f>DEC2HEX(G29)</f>
-        <v>869</v>
+        <v>86E</v>
       </c>
       <c r="J30" t="str">
         <f>DEC2HEX(J29)</f>
-        <v>515DE</v>
+        <v>51607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed period calcs for 57MHz pixel clock
</commit_message>
<xml_diff>
--- a/calculations/period_calculation.xlsx
+++ b/calculations/period_calculation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Galen\Documents\Code\miniscope_cypress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Documents\FEE\code\cyfxuvc_an75779\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -423,40 +423,39 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.53515625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="3" max="5" width="8.69140625" customWidth="1"/>
+    <col min="6" max="6" width="14.3046875" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" customWidth="1"/>
+    <col min="8" max="8" width="27.69140625" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="10" max="1025" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <f>113.75/2</f>
-        <v>56.875</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <f>10^9/(B1*10^6)</f>
-        <v>17.582417582417584</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17.543859649122808</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -468,25 +467,25 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6">
         <f>B2*C3*8/1000</f>
-        <v>15.472527472527474</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15.43859649122807</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
         <f>B6*(57/12)</f>
-        <v>73.494505494505503</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73.333333333333329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -496,32 +495,32 @@
       </c>
       <c r="C8">
         <f>C9/(B6*10^-6)</f>
-        <v>2154.3560606060605</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2159.090909090909</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
         <f>B8*B7/10^6</f>
-        <v>5.0123252747252753E-2</v>
+        <v>5.0013333333333326E-2</v>
       </c>
       <c r="C9">
         <f>1/C10</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B10">
         <f>1/B9</f>
-        <v>19.950820132175277</v>
+        <v>19.994668088509734</v>
       </c>
       <c r="C10">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -529,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -537,7 +536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -545,7 +544,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -553,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -563,14 +562,14 @@
       </c>
       <c r="C17">
         <f>B17*B6*10^-6</f>
-        <v>7.6589010989010992E-3</v>
+        <v>7.6421052631578945E-3</v>
       </c>
       <c r="D17">
         <f>1/C17</f>
-        <v>130.56703397612489</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>130.85399449035813</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -578,7 +577,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -586,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -594,7 +593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -602,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -611,7 +610,7 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -620,7 +619,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -630,28 +629,28 @@
       </c>
       <c r="C26">
         <f>B26*B6*10^-6</f>
-        <v>3.3405186813186813E-2</v>
+        <v>3.3331929824561402E-2</v>
       </c>
       <c r="D26">
         <f>1/C26</f>
-        <v>29.935470967198619</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30.001263211082573</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C27">
         <f>C26*10^9/100</f>
-        <v>334051.86813186813</v>
+        <v>333319.29824561405</v>
       </c>
       <c r="D27">
         <f>ROUND(C27,0)</f>
-        <v>334052</v>
+        <v>333319</v>
       </c>
       <c r="E27" t="str">
         <f>DEC2HEX(D27)</f>
-        <v>518E4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51607</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C28" t="s">
         <v>18</v>
       </c>
@@ -671,7 +670,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C29">
         <v>30</v>
       </c>
@@ -681,41 +680,41 @@
       </c>
       <c r="E29">
         <f>D29/(B6*10^-6)</f>
-        <v>2154.3560606060605</v>
+        <v>2159.090909090909</v>
       </c>
       <c r="F29">
         <f>ROUNDDOWN(E29,0)</f>
-        <v>2154</v>
+        <v>2159</v>
       </c>
       <c r="G29">
         <f>F29-1</f>
-        <v>2153</v>
+        <v>2158</v>
       </c>
       <c r="H29">
         <f>F29*B6*10^-6</f>
-        <v>3.3327824175824174E-2</v>
+        <v>3.3331929824561402E-2</v>
       </c>
       <c r="I29">
         <f>H29/10^-7</f>
-        <v>333278.24175824173</v>
+        <v>333319.29824561405</v>
       </c>
       <c r="J29">
         <f>ROUND(I29,0)</f>
-        <v>333278</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>333319</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="F30" t="str">
         <f>DEC2HEX(F29)</f>
-        <v>86A</v>
+        <v>86F</v>
       </c>
       <c r="G30" t="str">
         <f>DEC2HEX(G29)</f>
-        <v>869</v>
+        <v>86E</v>
       </c>
       <c r="J30" t="str">
         <f>DEC2HEX(J29)</f>
-        <v>515DE</v>
+        <v>51607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed frame period and max frame rate
</commit_message>
<xml_diff>
--- a/calculations/period_calculation.xlsx
+++ b/calculations/period_calculation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>clock (mhz)</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>rounded</t>
+  </si>
+  <si>
+    <t>bit rate/s</t>
+  </si>
+  <si>
+    <t>0xA53C000</t>
   </si>
 </sst>
 </file>
@@ -438,7 +444,7 @@
     <col min="10" max="1025" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +452,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -455,7 +461,7 @@
         <v>17.543859649122808</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -467,7 +473,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -475,8 +481,14 @@
         <f>B2*C3*8/1000</f>
         <v>15.43859649122807</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -484,8 +496,14 @@
         <f>B6*(57/12)</f>
         <v>73.333333333333329</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7">
+        <v>173260800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -497,8 +515,12 @@
         <f>C9/(B6*10^-6)</f>
         <v>2159.090909090909</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="I8">
+        <f>16*752*480*30</f>
+        <v>173260800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -511,7 +533,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B10">
         <f>1/B9</f>
         <v>19.994668088509734</v>
@@ -520,7 +542,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -528,7 +550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -536,7 +558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -544,7 +566,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>9</v>
       </c>

</xml_diff>